<commit_message>
final first round bracket results
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Judge</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>1H28</t>
+  </si>
+  <si>
+    <t>1I21</t>
+  </si>
+  <si>
+    <t>1I29</t>
+  </si>
+  <si>
+    <t>1I30</t>
   </si>
 </sst>
 </file>
@@ -932,15 +941,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1">
+    <row r="1" spans="1:37" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1025,17 @@
       <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AI1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1093,8 +1111,17 @@
       <c r="AG3">
         <v>3.1</v>
       </c>
+      <c r="AI3">
+        <v>3.1</v>
+      </c>
+      <c r="AJ3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AK3">
+        <v>1.0009999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1170,8 +1197,17 @@
       <c r="AG4">
         <v>3.1</v>
       </c>
+      <c r="AI4">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AJ4">
+        <v>3.1</v>
+      </c>
+      <c r="AK4">
+        <v>1.0009999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1247,8 +1283,17 @@
       <c r="AG5">
         <v>2.0099999999999998</v>
       </c>
+      <c r="AI5">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AJ5">
+        <v>3.1</v>
+      </c>
+      <c r="AK5">
+        <v>1.0009999999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1324,8 +1369,17 @@
       <c r="AG6">
         <v>1.0009999999999999</v>
       </c>
+      <c r="AI6">
+        <v>3.1</v>
+      </c>
+      <c r="AJ6">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="AK6">
+        <v>2.0099999999999998</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1420,7 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1407,7 +1461,7 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1416,7 +1470,7 @@
         <v>9.129999999999999</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:AG10" si="0">SUM(D3:D8)</f>
+        <f t="shared" ref="D10:AK10" si="0">SUM(D3:D8)</f>
         <v>9.2110000000000003</v>
       </c>
       <c r="E10">
@@ -1506,6 +1560,18 @@
       <c r="AG10">
         <f t="shared" si="0"/>
         <v>9.2110000000000003</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="0"/>
+        <v>10.219999999999999</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="0"/>
+        <v>9.2109999999999985</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="0"/>
+        <v>5.0129999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>